<commit_message>
new analysis excel file
</commit_message>
<xml_diff>
--- a/data/Supported Graphene Analysis.xlsx
+++ b/data/Supported Graphene Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinkrempl/Documents/TRI ORR/Data/DFT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F8E1FE9-261D-024C-B359-B3F7A8B726C5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF91AC9-A8ED-8041-992E-8A2DDD087076}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{4048BA77-A555-4A4B-8B58-A70623B0558E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="5" xr2:uid="{4048BA77-A555-4A4B-8B58-A70623B0558E}"/>
   </bookViews>
   <sheets>
     <sheet name="Lattice matching" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="vacuum" sheetId="4" r:id="rId3"/>
     <sheet name="layers" sheetId="5" r:id="rId4"/>
     <sheet name="pwcutoff " sheetId="3" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="46">
   <si>
     <t>001</t>
   </si>
@@ -115,9 +116,6 @@
     <t>elec.e out</t>
   </si>
   <si>
-    <t>bader failed</t>
-  </si>
-  <si>
     <t>bader per C</t>
   </si>
   <si>
@@ -145,9 +143,6 @@
     <t>elec.e out dipole on</t>
   </si>
   <si>
-    <t>bulk bader weird</t>
-  </si>
-  <si>
     <t>check bulk magmoms</t>
   </si>
   <si>
@@ -158,12 +153,31 @@
   </si>
   <si>
     <t>layers</t>
+  </si>
+  <si>
+    <t>dG ads</t>
+  </si>
+  <si>
+    <t>2x2</t>
+  </si>
+  <si>
+    <t>pw cutoff</t>
+  </si>
+  <si>
+    <t>4x4</t>
+  </si>
+  <si>
+    <t>2x2 trifold ontop</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.00000000000000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -201,16 +215,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,7 +545,7 @@
   <dimension ref="B2:L47"/>
   <sheetViews>
     <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -598,22 +614,22 @@
       <c r="E5">
         <v>0.01</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="3">
         <v>2.4901187</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="3">
         <v>2.4901187</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="3">
         <v>5.2660084653072703</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="4">
         <v>-8.9264542162520392E-3</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="4">
         <v>-8.9264542162524798E-3</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="5">
         <v>59.999999999999901</v>
       </c>
     </row>
@@ -630,22 +646,22 @@
       <c r="E6">
         <v>0.01</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="3">
         <v>6.4609920000000001</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="3">
         <v>19.255064099999998</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="3">
         <v>123.038432841599</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="4">
         <v>9.7765436880283794E-3</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="4">
         <v>1.6484513939999099E-2</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="5">
         <v>0.29264690570200003</v>
       </c>
     </row>
@@ -662,22 +678,22 @@
       <c r="E7">
         <v>0.01</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="3">
         <v>2.4901187</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="3">
         <v>23.284424699999999</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="3">
         <v>57.8514608956351</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="4">
         <v>-8.9264542162524798E-3</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="4">
         <v>1.02541519206751E-2</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="5">
         <v>5.8201933957306502E-2</v>
       </c>
     </row>
@@ -694,22 +710,22 @@
       <c r="E8">
         <v>0.01</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="3">
         <v>4.3095299999999996</v>
       </c>
       <c r="G8">
         <v>12.3626</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="3">
         <v>52.660084653072602</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="4">
         <v>-8.9264542162528198E-3</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="4">
         <v>-2.6806572059039301E-3</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="5">
         <v>1.4210854715202001E-14</v>
       </c>
     </row>
@@ -726,22 +742,22 @@
       <c r="E9">
         <v>0.01</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="3">
         <v>10.548054199999999</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="3">
         <v>21.096108399999999</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="3">
         <v>217.019396667997</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="4">
         <v>1.9013430954116999E-2</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="4">
         <v>-1.3011676374505799E-3</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9" s="5">
         <v>0.36505132780217697</v>
       </c>
     </row>
@@ -749,12 +765,12 @@
       <c r="B10" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B11">
@@ -769,22 +785,22 @@
       <c r="E11">
         <v>0.01</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="3">
         <v>4.98942</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="3">
         <v>29.936520000000002</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="3">
         <v>147.44823702860299</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11" s="4">
         <v>-1.1548436491616699E-2</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11" s="4">
         <v>-1.3051415231738401E-3</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11" s="3">
         <v>0</v>
       </c>
     </row>
@@ -801,22 +817,22 @@
       <c r="E12">
         <v>0.01</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="3">
         <v>8.6419288999999999</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="3">
         <v>12.2215331</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="3">
         <v>105.320169306145</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12" s="4">
         <v>-1.15484364916169E-2</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J12" s="4">
         <v>8.8341525215758204E-3</v>
       </c>
-      <c r="K12" s="2">
+      <c r="K12" s="3">
         <v>2.8421709430404001E-14</v>
       </c>
     </row>
@@ -833,22 +849,22 @@
       <c r="E13">
         <v>0.01</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="3">
         <v>4.98942</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="3">
         <v>4.98942</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="3">
         <v>21.064033861228999</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I13" s="4">
         <v>-1.15484364916162E-2</v>
       </c>
-      <c r="J13" s="3">
+      <c r="J13" s="4">
         <v>-1.1548436491616401E-2</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K13" s="3">
         <v>0</v>
       </c>
     </row>
@@ -865,22 +881,22 @@
       <c r="E14">
         <v>0.01</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="3">
         <v>4.98942</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="3">
         <v>29.936520000000002</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="3">
         <v>147.44823702860299</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14" s="4">
         <v>-1.15484364916169E-2</v>
       </c>
-      <c r="J14" s="3">
+      <c r="J14" s="4">
         <v>-1.30514152317395E-3</v>
       </c>
-      <c r="K14" s="2">
+      <c r="K14" s="3">
         <v>1.4210854715202001E-14</v>
       </c>
     </row>
@@ -897,22 +913,22 @@
       <c r="E15">
         <v>0.01</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="3">
         <v>4.98942</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="3">
         <v>51.490234200000003</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="3">
         <v>252.76840633474899</v>
       </c>
-      <c r="I15" s="3">
+      <c r="I15" s="4">
         <v>-1.15484364916162E-2</v>
       </c>
-      <c r="J15" s="3">
+      <c r="J15" s="4">
         <v>-3.4604455068828399E-3</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K15" s="3">
         <v>2.25564187795868E-2</v>
       </c>
     </row>
@@ -929,22 +945,22 @@
       <c r="E16">
         <v>0.01</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="3">
         <v>4.98942</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="3">
         <v>46.804908400000002</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="3">
         <v>231.70437247351899</v>
       </c>
-      <c r="I16" s="3">
+      <c r="I16" s="4">
         <v>-1.15484364916176E-2</v>
       </c>
-      <c r="J16" s="3">
+      <c r="J16" s="4">
         <v>3.7773078830720601E-3</v>
       </c>
-      <c r="K16" s="2">
+      <c r="K16" s="3">
         <v>4.2632564145605999E-14</v>
       </c>
     </row>
@@ -952,12 +968,12 @@
       <c r="B17" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="2"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="3"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18">
@@ -972,22 +988,22 @@
       <c r="E18">
         <v>0.01</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="3">
         <v>8.6347573000000004</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="3">
         <v>17.2695145</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="3">
         <v>147.44823702860299</v>
       </c>
-      <c r="I18" s="3">
+      <c r="I18" s="4">
         <v>-1.0727469153108699E-2</v>
       </c>
-      <c r="J18" s="3">
+      <c r="J18" s="4">
         <v>-4.7566652387964699E-4</v>
       </c>
-      <c r="K18" s="2">
+      <c r="K18" s="3">
         <v>2.8421709430404001E-14</v>
       </c>
     </row>
@@ -1004,22 +1020,22 @@
       <c r="E19">
         <v>0.01</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="3">
         <v>18.112400000000001</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" s="3">
         <v>19.3079</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H19" s="3">
         <v>315.96050791843601</v>
       </c>
-      <c r="I19" s="3">
+      <c r="I19" s="4">
         <v>-1.82505633592384E-2</v>
       </c>
-      <c r="J19" s="3">
+      <c r="J19" s="4">
         <v>1.3702691770434299E-2</v>
       </c>
-      <c r="K19" s="2">
+      <c r="K19" s="3">
         <v>0.44812092353400601</v>
       </c>
     </row>
@@ -1036,22 +1052,22 @@
       <c r="E20">
         <v>0.01</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="3">
         <v>10.9222</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="3">
         <v>10.9222</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20" s="3">
         <v>100.05416084083799</v>
       </c>
-      <c r="I20" s="3">
+      <c r="I20" s="4">
         <v>-1.5893418461761701E-2</v>
       </c>
-      <c r="J20" s="3">
+      <c r="J20" s="4">
         <v>-1.5893418461761899E-2</v>
       </c>
-      <c r="K20" s="2">
+      <c r="K20" s="3">
         <v>2.1316282072802999E-14</v>
       </c>
     </row>
@@ -1068,22 +1084,22 @@
       <c r="E21">
         <v>0.01</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="3">
         <v>10.9222</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21" s="3">
         <v>24.726099999999999</v>
       </c>
-      <c r="H21" s="2">
+      <c r="H21" s="3">
         <v>263.30042326536301</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I21" s="4">
         <v>-1.5893418461761899E-2</v>
       </c>
-      <c r="J21" s="3">
+      <c r="J21" s="4">
         <v>-2.717034487689E-3</v>
       </c>
-      <c r="K21" s="2">
+      <c r="K21" s="3">
         <v>0.24658380771960201</v>
       </c>
     </row>
@@ -1100,22 +1116,22 @@
       <c r="E22">
         <v>0.01</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="3">
         <v>10.9222</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22" s="3">
         <v>33.885199999999998</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H22" s="3">
         <v>363.35458410619998</v>
       </c>
-      <c r="I22" s="3">
+      <c r="I22" s="4">
         <v>-1.5893418461762399E-2</v>
       </c>
-      <c r="J22" s="3">
+      <c r="J22" s="4">
         <v>4.5110635345490998E-4</v>
       </c>
-      <c r="K22" s="2">
+      <c r="K22" s="3">
         <v>0.31541783033580301</v>
       </c>
     </row>
@@ -1132,22 +1148,22 @@
       <c r="E23">
         <v>0.01</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="3">
         <v>13.923126999999999</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23" s="3">
         <v>20.795248999999998</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H23" s="3">
         <v>279.09844866128299</v>
       </c>
-      <c r="I23" s="3">
+      <c r="I23" s="4">
         <v>-1.39033121187045E-2</v>
       </c>
-      <c r="J23" s="3">
+      <c r="J23" s="4">
         <v>1.31476943613164E-2</v>
       </c>
-      <c r="K23" s="2">
+      <c r="K23" s="3">
         <v>0.31164939805302</v>
       </c>
     </row>
@@ -1155,12 +1171,12 @@
       <c r="B24" t="s">
         <v>15</v>
       </c>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="2"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="3"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
@@ -1175,22 +1191,22 @@
       <c r="E25">
         <v>0.01</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F25" s="3">
         <v>9.8725400000000008</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G25" s="3">
         <v>9.8725400000000008</v>
       </c>
-      <c r="H25" s="2">
+      <c r="H25" s="3">
         <v>84.256135444916296</v>
       </c>
-      <c r="I25" s="3">
+      <c r="I25" s="4">
         <v>-9.0556479974235305E-4</v>
       </c>
-      <c r="J25" s="3">
+      <c r="J25" s="4">
         <v>-9.0556479974246396E-4</v>
       </c>
-      <c r="K25" s="2">
+      <c r="K25" s="3">
         <v>59.999999999999901</v>
       </c>
     </row>
@@ -1207,22 +1223,22 @@
       <c r="E26">
         <v>0.01</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F26" s="3">
         <v>4.28064</v>
       </c>
-      <c r="G26" s="2">
+      <c r="G26" s="3">
         <v>21.905200000000001</v>
       </c>
-      <c r="H26" s="2">
+      <c r="H26" s="3">
         <v>93.768275327999902</v>
       </c>
-      <c r="I26" s="3">
+      <c r="I26" s="4">
         <v>-2.23702848543783E-3</v>
       </c>
-      <c r="J26" s="3">
+      <c r="J26" s="4">
         <v>1.3142998009604501E-2</v>
       </c>
-      <c r="K26" s="2">
+      <c r="K26" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1239,22 +1255,22 @@
       <c r="E27">
         <v>0.01</v>
       </c>
-      <c r="F27" s="2">
+      <c r="F27" s="3">
         <v>13.2578525</v>
       </c>
-      <c r="G27" s="2">
+      <c r="G27" s="3">
         <v>16.1982085</v>
       </c>
-      <c r="H27" s="2">
+      <c r="H27" s="3">
         <v>210.64033861229001</v>
       </c>
-      <c r="I27" s="3">
+      <c r="I27" s="4">
         <v>-1.5804684474156699E-2</v>
       </c>
-      <c r="J27" s="3">
+      <c r="J27" s="4">
         <v>-1.74222223144293E-3</v>
       </c>
-      <c r="K27" s="2">
+      <c r="K27" s="3">
         <v>3.4038896278175898E-2</v>
       </c>
     </row>
@@ -1271,22 +1287,22 @@
       <c r="E28">
         <v>0.01</v>
       </c>
-      <c r="F28" s="2">
+      <c r="F28" s="3">
         <v>10.9526</v>
       </c>
-      <c r="G28" s="2">
+      <c r="G28" s="3">
         <v>13.067615</v>
       </c>
-      <c r="H28" s="2">
+      <c r="H28" s="3">
         <v>136.916220097989</v>
       </c>
-      <c r="I28" s="3">
+      <c r="I28" s="4">
         <v>-1.8624901404510601E-2</v>
       </c>
-      <c r="J28" s="3">
+      <c r="J28" s="4">
         <v>-1.47684445291496E-3</v>
       </c>
-      <c r="K28" s="2">
+      <c r="K28" s="3">
         <v>0.42460410656207098</v>
       </c>
     </row>
@@ -1303,22 +1319,22 @@
       <c r="E29">
         <v>0.01</v>
       </c>
-      <c r="F29" s="2">
+      <c r="F29" s="3">
         <v>13.257849999999999</v>
       </c>
-      <c r="G29" s="2">
+      <c r="G29" s="3">
         <v>18.591999999999999</v>
       </c>
-      <c r="H29" s="2">
+      <c r="H29" s="3">
         <v>231.70437247351899</v>
       </c>
-      <c r="I29" s="3">
+      <c r="I29" s="4">
         <v>-1.5804684474156099E-2</v>
       </c>
-      <c r="J29" s="3">
+      <c r="J29" s="4">
         <v>1.3493320800772499E-3</v>
       </c>
-      <c r="K29" s="2">
+      <c r="K29" s="3">
         <v>0.18129308995007401</v>
       </c>
     </row>
@@ -1326,12 +1342,12 @@
       <c r="B30" t="s">
         <v>16</v>
       </c>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="2"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="3"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B31">
@@ -1346,22 +1362,22 @@
       <c r="E31">
         <v>0.01</v>
       </c>
-      <c r="F31" s="2">
+      <c r="F31" s="3">
         <v>12.644</v>
       </c>
-      <c r="G31" s="2">
+      <c r="G31" s="3">
         <v>17.022600000000001</v>
       </c>
-      <c r="H31" s="2">
+      <c r="H31" s="3">
         <v>199.84150831259601</v>
       </c>
-      <c r="I31" s="3">
+      <c r="I31" s="4">
         <v>1.3373398643921E-2</v>
       </c>
-      <c r="J31" s="3">
+      <c r="J31" s="4">
         <v>1.40203016135043E-2</v>
       </c>
-      <c r="K31" s="2">
+      <c r="K31" s="3">
         <v>1.462018809E-2</v>
       </c>
     </row>
@@ -1378,22 +1394,22 @@
       <c r="E32">
         <v>0.01</v>
       </c>
-      <c r="F32" s="2">
+      <c r="F32" s="3">
         <v>13.033200000000001</v>
       </c>
-      <c r="G32" s="2">
+      <c r="G32" s="3">
         <v>16.4251</v>
       </c>
-      <c r="H32" s="2">
+      <c r="H32" s="3">
         <v>205.374330146983</v>
       </c>
-      <c r="I32" s="3">
+      <c r="I32" s="4">
         <v>-1.6883397458812399E-2</v>
       </c>
-      <c r="J32" s="3">
+      <c r="J32" s="4">
         <v>-1.55357387006681E-2</v>
       </c>
-      <c r="K32" s="2">
+      <c r="K32" s="3">
         <v>0.46037750655330001</v>
       </c>
     </row>
@@ -1410,22 +1426,22 @@
       <c r="E33">
         <v>0.01</v>
       </c>
-      <c r="F33" s="2">
+      <c r="F33" s="3">
         <v>8.9407200000000007</v>
       </c>
-      <c r="G33" s="2">
+      <c r="G33" s="3">
         <v>8.9407200000000007</v>
       </c>
-      <c r="H33" s="2">
+      <c r="H33" s="3">
         <v>68.458110048994499</v>
       </c>
-      <c r="I33" s="3">
+      <c r="I33" s="4">
         <v>-5.5698305421072397E-3</v>
       </c>
-      <c r="J33" s="3">
+      <c r="J33" s="4">
         <v>-5.5698305421072397E-3</v>
       </c>
-      <c r="K33" s="2">
+      <c r="K33" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1442,22 +1458,22 @@
       <c r="E34">
         <v>0.01</v>
       </c>
-      <c r="F34" s="2">
+      <c r="F34" s="3">
         <v>14.826000000000001</v>
       </c>
-      <c r="G34" s="2">
+      <c r="G34" s="3">
         <v>19.485800000000001</v>
       </c>
-      <c r="H34" s="2">
+      <c r="H34" s="3">
         <v>284.36445712659201</v>
       </c>
-      <c r="I34" s="3">
+      <c r="I34" s="4">
         <v>-2.0988595370090499E-3</v>
       </c>
-      <c r="J34" s="3">
+      <c r="J34" s="4">
         <v>-1.1627329561456999E-2</v>
       </c>
-      <c r="K34" s="2">
+      <c r="K34" s="3">
         <v>0.295902728782934</v>
       </c>
     </row>
@@ -1474,22 +1490,22 @@
       <c r="E35">
         <v>0.01</v>
       </c>
-      <c r="F35" s="2">
+      <c r="F35" s="3">
         <v>13.77858</v>
       </c>
-      <c r="G35" s="2">
+      <c r="G35" s="3">
         <v>19.485800000000001</v>
       </c>
-      <c r="H35" s="2">
+      <c r="H35" s="3">
         <v>258.03441480005603</v>
       </c>
-      <c r="I35" s="3">
+      <c r="I35" s="4">
         <v>-3.5588473568554102E-3</v>
       </c>
-      <c r="J35" s="3">
+      <c r="J35" s="4">
         <v>-1.16273295614571E-2</v>
       </c>
-      <c r="K35" s="2">
+      <c r="K35" s="3">
         <v>0.28397659492400001</v>
       </c>
     </row>
@@ -1506,22 +1522,22 @@
       <c r="E36">
         <v>0.01</v>
       </c>
-      <c r="F36" s="2">
+      <c r="F36" s="3">
         <v>9.9960000000000004</v>
       </c>
-      <c r="G36" s="2">
+      <c r="G36" s="3">
         <v>22.35181</v>
       </c>
-      <c r="H36" s="2">
+      <c r="H36" s="3">
         <v>210.64033861229001</v>
       </c>
-      <c r="I36" s="3">
+      <c r="I36" s="4">
         <v>-1.3248942910312001E-2</v>
       </c>
-      <c r="J36" s="3">
+      <c r="J36" s="4">
         <v>-1.9435530901065302E-2</v>
       </c>
-      <c r="K36" s="2">
+      <c r="K36" s="3">
         <v>8.2945561239171101E-2</v>
       </c>
     </row>
@@ -1538,22 +1554,22 @@
       <c r="E37">
         <v>0.01</v>
       </c>
-      <c r="F37" s="2">
+      <c r="F37" s="3">
         <v>17.021999999999998</v>
       </c>
-      <c r="G37" s="2">
+      <c r="G37" s="3">
         <v>17.021999999999998</v>
       </c>
-      <c r="H37" s="2">
+      <c r="H37" s="3">
         <v>281.201928016887</v>
       </c>
-      <c r="I37" s="3">
+      <c r="I37" s="4">
         <v>1.4020301613502499E-2</v>
       </c>
-      <c r="J37" s="3">
+      <c r="J37" s="4">
         <v>1.4020301613501601E-2</v>
       </c>
-      <c r="K37" s="2">
+      <c r="K37" s="3">
         <v>0.39438407812769999</v>
       </c>
     </row>
@@ -1561,12 +1577,12 @@
       <c r="B38" t="s">
         <v>17</v>
       </c>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="2"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="3"/>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B39">
@@ -1581,22 +1597,22 @@
       <c r="E39">
         <v>0.01</v>
       </c>
-      <c r="F39" s="2">
+      <c r="F39" s="3">
         <v>9.0009999999999994</v>
       </c>
-      <c r="G39" s="2">
+      <c r="G39" s="3">
         <v>15.913</v>
       </c>
-      <c r="H39" s="2">
+      <c r="H39" s="3">
         <v>141.807776767836</v>
       </c>
-      <c r="I39" s="3">
+      <c r="I39" s="4">
         <v>-1.23202789700529E-2</v>
       </c>
-      <c r="J39" s="3">
+      <c r="J39" s="4">
         <v>1.61403046351795E-2</v>
       </c>
-      <c r="K39" s="2">
+      <c r="K39" s="3">
         <v>0.38292192885509702</v>
       </c>
     </row>
@@ -1613,22 +1629,22 @@
       <c r="E40">
         <v>0.01</v>
       </c>
-      <c r="F40" s="2">
+      <c r="F40" s="3">
         <v>12.73</v>
       </c>
-      <c r="G40" s="2">
+      <c r="G40" s="3">
         <v>14.927852</v>
       </c>
-      <c r="H40" s="2">
+      <c r="H40" s="3">
         <v>171.89698384718599</v>
       </c>
-      <c r="I40" s="3">
+      <c r="I40" s="4">
         <v>6.4943586912951101E-3</v>
       </c>
-      <c r="J40" s="3">
+      <c r="J40" s="4">
         <v>4.7984950457298199E-3</v>
       </c>
-      <c r="K40" s="2">
+      <c r="K40" s="3">
         <v>4.5594225372795401E-2</v>
       </c>
     </row>
@@ -1645,22 +1661,22 @@
       <c r="E41">
         <v>0.01</v>
       </c>
-      <c r="F41" s="2">
+      <c r="F41" s="3">
         <v>9.0018340000000006</v>
       </c>
-      <c r="G41" s="2">
+      <c r="G41" s="3">
         <v>9.0018340000000006</v>
       </c>
-      <c r="H41" s="2">
+      <c r="H41" s="3">
         <v>68.458110048994499</v>
       </c>
-      <c r="I41" s="3">
+      <c r="I41" s="4">
         <v>-1.23202789700535E-2</v>
       </c>
-      <c r="J41" s="3">
+      <c r="J41" s="4">
         <v>-1.23202789700533E-2</v>
       </c>
-      <c r="K41" s="2">
+      <c r="K41" s="3">
         <v>59.999999999999901</v>
       </c>
     </row>
@@ -1677,22 +1693,22 @@
       <c r="E42">
         <v>0.01</v>
       </c>
-      <c r="F42" s="2">
+      <c r="F42" s="3">
         <v>17.138000000000002</v>
       </c>
-      <c r="G42" s="2">
+      <c r="G42" s="3">
         <v>18.828600000000002</v>
       </c>
-      <c r="H42" s="2">
+      <c r="H42" s="3">
         <v>321.22651638374299</v>
       </c>
-      <c r="I42" s="3">
+      <c r="I42" s="4">
         <v>7.1368703167005096E-3</v>
       </c>
-      <c r="J42" s="3">
+      <c r="J42" s="4">
         <v>-1.12355123377465E-2</v>
       </c>
-      <c r="K42" s="2">
+      <c r="K42" s="3">
         <v>0.172274026209251</v>
       </c>
     </row>
@@ -1709,22 +1725,22 @@
       <c r="E43">
         <v>0.01</v>
       </c>
-      <c r="F43" s="2">
+      <c r="F43" s="3">
         <v>13.872</v>
       </c>
-      <c r="G43" s="2">
+      <c r="G43" s="3">
         <v>19.619</v>
       </c>
-      <c r="H43" s="2">
+      <c r="H43" s="3">
         <v>258.03441480005603</v>
       </c>
-      <c r="I43" s="3">
+      <c r="I43" s="4">
         <v>-1.0322946857242599E-2</v>
       </c>
-      <c r="J43" s="3">
+      <c r="J43" s="4">
         <v>-1.8336658123988499E-2</v>
       </c>
-      <c r="K43" s="2">
+      <c r="K43" s="3">
         <v>0.283976594924226</v>
       </c>
     </row>
@@ -1741,22 +1757,22 @@
       <c r="E44">
         <v>0.01</v>
       </c>
-      <c r="F44" s="2">
+      <c r="F44" s="3">
         <v>9.00183</v>
       </c>
-      <c r="G44" s="2">
+      <c r="G44" s="3">
         <v>39.238079999999997</v>
       </c>
-      <c r="H44" s="2">
+      <c r="H44" s="3">
         <v>352.82256717558499</v>
       </c>
-      <c r="I44" s="3">
+      <c r="I44" s="4">
         <v>-1.2320278970055901E-2</v>
       </c>
-      <c r="J44" s="3">
+      <c r="J44" s="4">
         <v>1.1387408234965601E-2</v>
       </c>
-      <c r="K44" s="2">
+      <c r="K44" s="3">
         <v>0.49371514890667301</v>
       </c>
     </row>
@@ -1773,40 +1789,40 @@
       <c r="E45">
         <v>0.01</v>
       </c>
-      <c r="F45" s="2">
+      <c r="F45" s="3">
         <v>17.1389</v>
       </c>
-      <c r="G45" s="2">
+      <c r="G45" s="3">
         <v>17.1389</v>
       </c>
-      <c r="H45" s="2">
+      <c r="H45" s="3">
         <v>285.05889900745001</v>
       </c>
-      <c r="I45" s="3">
+      <c r="I45" s="4">
         <v>7.1368703166994002E-3</v>
       </c>
-      <c r="J45" s="3">
+      <c r="J45" s="4">
         <v>7.1368703166980697E-3</v>
       </c>
-      <c r="K45" s="2">
+      <c r="K45" s="3">
         <v>0.394384078127686</v>
       </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
-      <c r="K46" s="2"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="3"/>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
-      <c r="K47" s="2"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H5:H45">
@@ -1829,8 +1845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA11F605-3F2C-8949-A07B-2C4748B8A05E}">
   <dimension ref="B2:U92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q43" sqref="Q43"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1839,6 +1855,7 @@
     <col min="12" max="12" width="11.33203125" customWidth="1"/>
     <col min="13" max="13" width="14.5" customWidth="1"/>
     <col min="14" max="14" width="13.33203125" customWidth="1"/>
+    <col min="17" max="17" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1852,7 +1869,7 @@
         <v>331</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
         <v>24</v>
@@ -1864,31 +1881,31 @@
         <v>26</v>
       </c>
       <c r="H4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" t="s">
         <v>40</v>
       </c>
-      <c r="I4" t="s">
-        <v>42</v>
-      </c>
       <c r="K4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" t="s">
         <v>31</v>
       </c>
-      <c r="N4" t="s">
-        <v>32</v>
-      </c>
       <c r="O4" t="s">
+        <v>28</v>
+      </c>
+      <c r="P4" t="s">
         <v>29</v>
       </c>
-      <c r="P4" t="s">
-        <v>30</v>
-      </c>
       <c r="Q4" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.2">
@@ -1896,12 +1913,12 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5">
         <v>3</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="7">
         <v>1.9999999999999999E-7</v>
       </c>
       <c r="F5">
@@ -1932,9 +1949,13 @@
         <f>AVERAGE(M5:N5)</f>
         <v>-6.989999999999999E-2</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5" s="3">
         <f t="shared" ref="P5:P24" si="0">K6-K5</f>
         <v>-458.35122749999937</v>
+      </c>
+      <c r="Q5" s="8">
+        <f>K6-(K5-460.15205)</f>
+        <v>1.8008225000012317</v>
       </c>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.2">
@@ -1942,12 +1963,12 @@
         <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6">
         <v>5</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="7">
         <v>1.9999999999999999E-7</v>
       </c>
       <c r="F6">
@@ -1968,31 +1989,34 @@
       <c r="L6">
         <v>-25227.010756200001</v>
       </c>
-      <c r="P6" s="2"/>
-      <c r="R6" s="5"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="6"/>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="P7" s="2"/>
-      <c r="T7" s="5"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="8"/>
+      <c r="T7" s="6"/>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>441</v>
       </c>
-      <c r="P8" s="2"/>
-      <c r="T8" s="5"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="8"/>
+      <c r="T8" s="6"/>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9">
         <v>3</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="7">
         <v>1.9999999999999999E-7</v>
       </c>
       <c r="F9">
@@ -2023,27 +2047,28 @@
         <f t="shared" ref="O9:O24" si="1">AVERAGE(M9:N9)</f>
         <v>-6.3249999999999987E-2</v>
       </c>
-      <c r="P9" s="2">
+      <c r="P9" s="3">
         <f>K10-K9</f>
         <v>-458.82965360000162</v>
       </c>
-      <c r="Q9" t="s">
-        <v>38</v>
-      </c>
-      <c r="T9" s="5"/>
-      <c r="U9" s="5"/>
+      <c r="Q9" s="8">
+        <f t="shared" ref="Q6:Q39" si="2">K10-(K9-460.15205)</f>
+        <v>1.3223963999989792</v>
+      </c>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10">
         <v>3</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="7">
         <v>1.9999999999999999E-7</v>
       </c>
       <c r="F10">
@@ -2064,37 +2089,37 @@
       <c r="L10">
         <v>-25227.201683200001</v>
       </c>
-      <c r="P10" s="2"/>
-      <c r="Q10" t="s">
-        <v>28</v>
-      </c>
-      <c r="T10" s="5"/>
-      <c r="U10" s="5"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="8"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="P11" s="2"/>
-      <c r="T11" s="5"/>
-      <c r="U11" s="5"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="8"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>661</v>
       </c>
-      <c r="P12" s="2"/>
-      <c r="T12" s="5"/>
-      <c r="U12" s="5"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="8"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="6"/>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13">
         <v>2</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="7">
         <v>1.9999999999999999E-7</v>
       </c>
       <c r="F13">
@@ -2109,7 +2134,7 @@
       <c r="I13">
         <v>6</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K13" s="3">
         <v>-24768.9690018</v>
       </c>
       <c r="L13">
@@ -2125,24 +2150,28 @@
         <f t="shared" si="1"/>
         <v>-6.93E-2</v>
       </c>
-      <c r="P13" s="2">
+      <c r="P13" s="3">
         <f t="shared" si="0"/>
         <v>-458.38072390000161</v>
       </c>
-      <c r="T13" s="5"/>
-      <c r="U13" s="5"/>
+      <c r="Q13" s="8">
+        <f t="shared" si="2"/>
+        <v>1.771326099998987</v>
+      </c>
+      <c r="T13" s="6"/>
+      <c r="U13" s="6"/>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D14">
         <v>6</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="7">
         <v>1.9999999999999999E-7</v>
       </c>
       <c r="F14">
@@ -2163,34 +2192,37 @@
       <c r="L14">
         <v>-25227.349728900001</v>
       </c>
-      <c r="P14" s="2"/>
-      <c r="T14" s="5"/>
-      <c r="U14" s="5"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="8"/>
+      <c r="T14" s="6"/>
+      <c r="U14" s="6"/>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="P15" s="2"/>
-      <c r="T15" s="5"/>
-      <c r="U15" s="5"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="8"/>
+      <c r="T15" s="6"/>
+      <c r="U15" s="6"/>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B16">
         <v>881</v>
       </c>
-      <c r="P16" s="2"/>
-      <c r="T16" s="5"/>
-      <c r="U16" s="5"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="8"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D17">
         <v>6</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="7">
         <v>1.9999999999999999E-7</v>
       </c>
       <c r="F17">
@@ -2221,24 +2253,28 @@
         <f t="shared" si="1"/>
         <v>-6.3799999999999996E-2</v>
       </c>
-      <c r="P17" s="2">
+      <c r="P17" s="3">
         <f t="shared" si="0"/>
         <v>-458.42419820000214</v>
       </c>
-      <c r="T17" s="5"/>
-      <c r="U17" s="5"/>
+      <c r="Q17" s="8">
+        <f t="shared" si="2"/>
+        <v>1.7278517999984615</v>
+      </c>
+      <c r="T17" s="6"/>
+      <c r="U17" s="6"/>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D18">
         <v>3</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="7">
         <v>1.9999999999999999E-7</v>
       </c>
       <c r="F18">
@@ -2259,27 +2295,29 @@
       <c r="L18">
         <v>-25227.284586599999</v>
       </c>
-      <c r="P18" s="2"/>
-      <c r="T18" s="5"/>
-      <c r="U18" s="5"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="8"/>
+      <c r="T18" s="6"/>
+      <c r="U18" s="6"/>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="E19" s="6"/>
-      <c r="P19" s="2"/>
-      <c r="T19" s="5"/>
-      <c r="U19" s="5"/>
+      <c r="E19" s="7"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="8"/>
+      <c r="T19" s="6"/>
+      <c r="U19" s="6"/>
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="7">
         <v>1.9999999999999999E-7</v>
       </c>
       <c r="F20">
@@ -2307,24 +2345,28 @@
         <f t="shared" si="1"/>
         <v>-6.770000000000001E-2</v>
       </c>
-      <c r="P20" s="2">
+      <c r="P20" s="3">
         <f t="shared" si="0"/>
         <v>-458.43829080000069</v>
       </c>
-      <c r="T20" s="5"/>
-      <c r="U20" s="5"/>
+      <c r="Q20" s="8">
+        <f t="shared" si="2"/>
+        <v>1.7137591999999131</v>
+      </c>
+      <c r="T20" s="6"/>
+      <c r="U20" s="6"/>
     </row>
     <row r="21" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="7">
         <v>1.9999999999999999E-7</v>
       </c>
       <c r="F21">
@@ -2342,34 +2384,37 @@
       <c r="K21">
         <v>-13000.0954435</v>
       </c>
-      <c r="P21" s="2"/>
-      <c r="T21" s="5"/>
-      <c r="U21" s="5"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="8"/>
+      <c r="T21" s="6"/>
+      <c r="U21" s="6"/>
     </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="P22" s="2"/>
-      <c r="T22" s="5"/>
-      <c r="U22" s="5"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="8"/>
+      <c r="T22" s="6"/>
+      <c r="U22" s="6"/>
     </row>
     <row r="23" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B23">
         <v>10101</v>
       </c>
-      <c r="P23" s="2"/>
-      <c r="T23" s="5"/>
-      <c r="U23" s="5"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="8"/>
+      <c r="T23" s="6"/>
+      <c r="U23" s="6"/>
     </row>
     <row r="24" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>19</v>
       </c>
       <c r="C24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D24">
         <v>2</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="7">
         <v>1.9999999999999999E-7</v>
       </c>
       <c r="F24">
@@ -2400,24 +2445,28 @@
         <f t="shared" si="1"/>
         <v>-6.7250000000000004E-2</v>
       </c>
-      <c r="P24" s="2">
+      <c r="P24" s="3">
         <f t="shared" si="0"/>
         <v>-457.64924070000052</v>
       </c>
-      <c r="T24" s="5"/>
-      <c r="U24" s="5"/>
+      <c r="Q24" s="8">
+        <f t="shared" si="2"/>
+        <v>2.5028093000000808</v>
+      </c>
+      <c r="T24" s="6"/>
+      <c r="U24" s="6"/>
     </row>
     <row r="25" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>20</v>
       </c>
       <c r="C25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D25">
         <v>4</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="7">
         <v>1.9999999999999999E-7</v>
       </c>
       <c r="F25">
@@ -2435,26 +2484,28 @@
       <c r="K25">
         <v>-25226.486600799999</v>
       </c>
-      <c r="P25" s="2"/>
-      <c r="T25" s="5"/>
-      <c r="U25" s="5"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="8"/>
+      <c r="T25" s="6"/>
+      <c r="U25" s="6"/>
     </row>
     <row r="26" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="P26" s="2"/>
-      <c r="T26" s="5"/>
-      <c r="U26" s="5"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="8"/>
+      <c r="T26" s="6"/>
+      <c r="U26" s="6"/>
     </row>
     <row r="27" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>19</v>
       </c>
       <c r="C27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D27">
         <v>3</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="7">
         <v>1.9999999999999999E-7</v>
       </c>
       <c r="F27">
@@ -2479,27 +2530,31 @@
         <v>-0.33929999999999999</v>
       </c>
       <c r="O27">
-        <f t="shared" ref="O27:O64" si="2">AVERAGE(M27:N27)</f>
+        <f t="shared" ref="O27:O64" si="3">AVERAGE(M27:N27)</f>
         <v>-6.1699999999999991E-2</v>
       </c>
-      <c r="P27" s="2">
-        <f t="shared" ref="P27:P64" si="3">K28-K27</f>
+      <c r="P27" s="3">
+        <f t="shared" ref="P27:P64" si="4">K28-K27</f>
         <v>-458.42866569999933</v>
       </c>
-      <c r="T27" s="5"/>
-      <c r="U27" s="5"/>
+      <c r="Q27" s="8">
+        <f t="shared" si="2"/>
+        <v>1.7233843000012712</v>
+      </c>
+      <c r="T27" s="6"/>
+      <c r="U27" s="6"/>
     </row>
     <row r="28" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>20</v>
       </c>
       <c r="C28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D28">
         <v>5</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="7">
         <v>1.9999999999999999E-7</v>
       </c>
       <c r="F28">
@@ -2517,34 +2572,37 @@
       <c r="K28">
         <v>-13000.0813186</v>
       </c>
-      <c r="P28" s="2"/>
-      <c r="T28" s="5"/>
-      <c r="U28" s="5"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="8"/>
+      <c r="T28" s="6"/>
+      <c r="U28" s="6"/>
     </row>
     <row r="29" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="P29" s="2"/>
-      <c r="T29" s="5"/>
-      <c r="U29" s="5"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="8"/>
+      <c r="T29" s="6"/>
+      <c r="U29" s="6"/>
     </row>
     <row r="30" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B30">
         <v>12121</v>
       </c>
-      <c r="P30" s="2"/>
-      <c r="T30" s="5"/>
-      <c r="U30" s="5"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="8"/>
+      <c r="T30" s="6"/>
+      <c r="U30" s="6"/>
     </row>
     <row r="31" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>21</v>
       </c>
       <c r="C31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="7">
         <v>1.9999999999999999E-7</v>
       </c>
       <c r="F31">
@@ -2569,27 +2627,31 @@
         <v>-0.33489999999999998</v>
       </c>
       <c r="O31">
+        <f t="shared" si="3"/>
+        <v>-5.8899999999999994E-2</v>
+      </c>
+      <c r="P31" s="3">
+        <f t="shared" si="4"/>
+        <v>-458.43399979999958</v>
+      </c>
+      <c r="Q31" s="8">
         <f t="shared" si="2"/>
-        <v>-5.8899999999999994E-2</v>
-      </c>
-      <c r="P31" s="2">
-        <f t="shared" si="3"/>
-        <v>-458.43399979999958</v>
-      </c>
-      <c r="T31" s="5"/>
-      <c r="U31" s="5"/>
+        <v>1.7180502000010165</v>
+      </c>
+      <c r="T31" s="6"/>
+      <c r="U31" s="6"/>
     </row>
     <row r="32" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>20</v>
       </c>
       <c r="C32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D32">
         <v>2</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E32" s="7">
         <v>1.9999999999999999E-7</v>
       </c>
       <c r="F32">
@@ -2607,34 +2669,37 @@
       <c r="K32">
         <v>-13000.067227</v>
       </c>
-      <c r="P32" s="2"/>
-      <c r="T32" s="5"/>
-      <c r="U32" s="5"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="8"/>
+      <c r="T32" s="6"/>
+      <c r="U32" s="6"/>
     </row>
     <row r="33" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="P33" s="2"/>
-      <c r="T33" s="5"/>
-      <c r="U33" s="5"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="8"/>
+      <c r="T33" s="6"/>
+      <c r="U33" s="6"/>
     </row>
     <row r="34" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B34">
         <v>16161</v>
       </c>
-      <c r="P34" s="2"/>
-      <c r="T34" s="5"/>
-      <c r="U34" s="5"/>
+      <c r="P34" s="3"/>
+      <c r="Q34" s="8"/>
+      <c r="T34" s="6"/>
+      <c r="U34" s="6"/>
     </row>
     <row r="35" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>19</v>
       </c>
       <c r="C35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D35">
         <v>1</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E35" s="7">
         <v>1.9999999999999999E-7</v>
       </c>
       <c r="F35">
@@ -2659,27 +2724,31 @@
         <v>-0.12479999999999999</v>
       </c>
       <c r="O35">
+        <f t="shared" si="3"/>
+        <v>-6.7500000000000004E-2</v>
+      </c>
+      <c r="P35" s="3">
+        <f t="shared" si="4"/>
+        <v>-458.45270160000109</v>
+      </c>
+      <c r="Q35" s="8">
         <f t="shared" si="2"/>
-        <v>-6.7500000000000004E-2</v>
-      </c>
-      <c r="P35" s="2">
-        <f t="shared" si="3"/>
-        <v>-458.45270160000109</v>
-      </c>
-      <c r="T35" s="5"/>
-      <c r="U35" s="5"/>
+        <v>1.6993483999995078</v>
+      </c>
+      <c r="T35" s="6"/>
+      <c r="U35" s="6"/>
     </row>
     <row r="36" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>20</v>
       </c>
       <c r="C36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D36">
         <v>3</v>
       </c>
-      <c r="E36" s="6">
+      <c r="E36" s="7">
         <v>1.9999999999999999E-7</v>
       </c>
       <c r="F36">
@@ -2697,34 +2766,37 @@
       <c r="K36">
         <v>-13000.0832656</v>
       </c>
-      <c r="P36" s="2"/>
-      <c r="T36" s="5"/>
-      <c r="U36" s="5"/>
+      <c r="P36" s="3"/>
+      <c r="Q36" s="8"/>
+      <c r="T36" s="6"/>
+      <c r="U36" s="6"/>
     </row>
     <row r="37" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="P37" s="2"/>
-      <c r="T37" s="5"/>
-      <c r="U37" s="5"/>
+      <c r="P37" s="3"/>
+      <c r="Q37" s="8"/>
+      <c r="T37" s="6"/>
+      <c r="U37" s="6"/>
     </row>
     <row r="38" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B38">
         <v>24241</v>
       </c>
-      <c r="P38" s="2"/>
-      <c r="T38" s="5"/>
-      <c r="U38" s="5"/>
+      <c r="P38" s="3"/>
+      <c r="Q38" s="8"/>
+      <c r="T38" s="6"/>
+      <c r="U38" s="6"/>
     </row>
     <row r="39" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>19</v>
       </c>
       <c r="C39" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D39">
         <v>2</v>
       </c>
-      <c r="E39" s="6">
+      <c r="E39" s="7">
         <v>1.9999999999999999E-7</v>
       </c>
       <c r="F39">
@@ -2749,27 +2821,31 @@
         <v>-0.33019999999999999</v>
       </c>
       <c r="O39">
+        <f t="shared" si="3"/>
+        <v>-6.2699999999999992E-2</v>
+      </c>
+      <c r="P39" s="3">
+        <f t="shared" si="4"/>
+        <v>-458.44683120000082</v>
+      </c>
+      <c r="Q39" s="8">
         <f t="shared" si="2"/>
-        <v>-6.2699999999999992E-2</v>
-      </c>
-      <c r="P39" s="2">
-        <f t="shared" si="3"/>
-        <v>-458.44683120000082</v>
-      </c>
-      <c r="T39" s="5"/>
-      <c r="U39" s="5"/>
+        <v>1.7052187999997841</v>
+      </c>
+      <c r="T39" s="6"/>
+      <c r="U39" s="6"/>
     </row>
     <row r="40" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>20</v>
       </c>
       <c r="C40" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D40">
         <v>1</v>
       </c>
-      <c r="E40" s="6">
+      <c r="E40" s="7">
         <v>1.9999999999999999E-7</v>
       </c>
       <c r="F40">
@@ -2787,53 +2863,53 @@
       <c r="K40">
         <v>-13000.0819097</v>
       </c>
-      <c r="T40" s="5"/>
-      <c r="U40" s="5"/>
+      <c r="T40" s="6"/>
+      <c r="U40" s="6"/>
     </row>
     <row r="41" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="T41" s="5"/>
-      <c r="U41" s="5"/>
+      <c r="T41" s="6"/>
+      <c r="U41" s="6"/>
     </row>
     <row r="42" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="T42" s="5"/>
-      <c r="U42" s="5"/>
+      <c r="T42" s="6"/>
+      <c r="U42" s="6"/>
     </row>
     <row r="43" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>39</v>
-      </c>
-      <c r="T43" s="5"/>
-      <c r="U43" s="5"/>
+        <v>37</v>
+      </c>
+      <c r="T43" s="6"/>
+      <c r="U43" s="6"/>
     </row>
     <row r="44" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="T44" s="5"/>
-      <c r="U44" s="5"/>
+      <c r="T44" s="6"/>
+      <c r="U44" s="6"/>
     </row>
     <row r="45" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="T45" s="5"/>
-      <c r="U45" s="5"/>
+      <c r="T45" s="6"/>
+      <c r="U45" s="6"/>
     </row>
     <row r="46" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="T46" s="5"/>
-      <c r="U46" s="5"/>
+      <c r="T46" s="6"/>
+      <c r="U46" s="6"/>
     </row>
     <row r="47" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>22</v>
       </c>
-      <c r="T47" s="5"/>
-      <c r="U47" s="5"/>
+      <c r="T47" s="6"/>
+      <c r="U47" s="6"/>
     </row>
     <row r="48" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="T48" s="5"/>
-      <c r="U48" s="5"/>
+      <c r="T48" s="6"/>
+      <c r="U48" s="6"/>
     </row>
     <row r="49" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B49">
         <v>331</v>
       </c>
-      <c r="T49" s="5"/>
-      <c r="U49" s="5"/>
+      <c r="T49" s="6"/>
+      <c r="U49" s="6"/>
     </row>
     <row r="50" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
@@ -2842,7 +2918,7 @@
       <c r="C50" t="s">
         <v>23</v>
       </c>
-      <c r="E50" s="6">
+      <c r="E50" s="7">
         <v>1.9999999999999999E-6</v>
       </c>
       <c r="F50">
@@ -2851,26 +2927,26 @@
       <c r="G50">
         <v>400</v>
       </c>
-      <c r="S50" s="5"/>
-      <c r="U50" s="5"/>
+      <c r="S50" s="6"/>
+      <c r="U50" s="6"/>
     </row>
     <row r="51" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>20</v>
       </c>
-      <c r="S51" s="5"/>
-      <c r="U51" s="5"/>
+      <c r="S51" s="6"/>
+      <c r="U51" s="6"/>
     </row>
     <row r="52" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="S52" s="5"/>
-      <c r="U52" s="5"/>
+      <c r="S52" s="6"/>
+      <c r="U52" s="6"/>
     </row>
     <row r="53" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B53">
         <v>441</v>
       </c>
-      <c r="S53" s="5"/>
-      <c r="U53" s="5"/>
+      <c r="S53" s="6"/>
+      <c r="U53" s="6"/>
     </row>
     <row r="54" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
@@ -2879,7 +2955,7 @@
       <c r="C54" t="s">
         <v>23</v>
       </c>
-      <c r="E54" s="6">
+      <c r="E54" s="7">
         <v>1.9999999999999999E-6</v>
       </c>
       <c r="F54">
@@ -2888,166 +2964,166 @@
       <c r="G54">
         <v>400</v>
       </c>
-      <c r="S54" s="5"/>
-      <c r="U54" s="5"/>
+      <c r="S54" s="6"/>
+      <c r="U54" s="6"/>
     </row>
     <row r="55" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>20</v>
       </c>
-      <c r="S55" s="5"/>
-      <c r="U55" s="5"/>
+      <c r="S55" s="6"/>
+      <c r="U55" s="6"/>
     </row>
     <row r="56" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="S56" s="5"/>
-      <c r="U56" s="5"/>
+      <c r="S56" s="6"/>
+      <c r="U56" s="6"/>
     </row>
     <row r="57" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="S57" s="5"/>
-      <c r="U57" s="5"/>
+      <c r="S57" s="6"/>
+      <c r="U57" s="6"/>
     </row>
     <row r="58" spans="2:21" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="S58" s="5"/>
-      <c r="U58" s="5"/>
+      <c r="S58" s="6"/>
+      <c r="U58" s="6"/>
     </row>
     <row r="59" spans="2:21" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="S59" s="5"/>
-      <c r="U59" s="5"/>
+      <c r="S59" s="6"/>
+      <c r="U59" s="6"/>
     </row>
     <row r="60" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="S60" s="5"/>
-      <c r="U60" s="5"/>
+      <c r="S60" s="6"/>
+      <c r="U60" s="6"/>
     </row>
     <row r="61" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="S61" s="5"/>
-      <c r="U61" s="5"/>
+      <c r="S61" s="6"/>
+      <c r="U61" s="6"/>
     </row>
     <row r="62" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="S62" s="5"/>
-      <c r="U62" s="5"/>
+      <c r="S62" s="6"/>
+      <c r="U62" s="6"/>
     </row>
     <row r="63" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="S63" s="5"/>
-      <c r="U63" s="5"/>
+      <c r="S63" s="6"/>
+      <c r="U63" s="6"/>
     </row>
     <row r="64" spans="2:21" x14ac:dyDescent="0.2">
       <c r="O64" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="P64">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="S64" s="5"/>
-      <c r="U64" s="5"/>
+      <c r="S64" s="6"/>
+      <c r="U64" s="6"/>
     </row>
     <row r="65" spans="19:21" x14ac:dyDescent="0.2">
-      <c r="S65" s="5"/>
-      <c r="U65" s="5"/>
+      <c r="S65" s="6"/>
+      <c r="U65" s="6"/>
     </row>
     <row r="66" spans="19:21" x14ac:dyDescent="0.2">
-      <c r="S66" s="5"/>
-      <c r="U66" s="5"/>
+      <c r="S66" s="6"/>
+      <c r="U66" s="6"/>
     </row>
     <row r="67" spans="19:21" x14ac:dyDescent="0.2">
-      <c r="S67" s="5"/>
-      <c r="U67" s="5"/>
+      <c r="S67" s="6"/>
+      <c r="U67" s="6"/>
     </row>
     <row r="68" spans="19:21" x14ac:dyDescent="0.2">
-      <c r="S68" s="5"/>
-      <c r="U68" s="5"/>
+      <c r="S68" s="6"/>
+      <c r="U68" s="6"/>
     </row>
     <row r="69" spans="19:21" x14ac:dyDescent="0.2">
-      <c r="S69" s="5"/>
-      <c r="U69" s="5"/>
+      <c r="S69" s="6"/>
+      <c r="U69" s="6"/>
     </row>
     <row r="70" spans="19:21" x14ac:dyDescent="0.2">
-      <c r="S70" s="5"/>
-      <c r="U70" s="5"/>
+      <c r="S70" s="6"/>
+      <c r="U70" s="6"/>
     </row>
     <row r="71" spans="19:21" x14ac:dyDescent="0.2">
-      <c r="S71" s="5"/>
-      <c r="U71" s="5"/>
+      <c r="S71" s="6"/>
+      <c r="U71" s="6"/>
     </row>
     <row r="72" spans="19:21" x14ac:dyDescent="0.2">
-      <c r="S72" s="5"/>
-      <c r="U72" s="5"/>
+      <c r="S72" s="6"/>
+      <c r="U72" s="6"/>
     </row>
     <row r="73" spans="19:21" x14ac:dyDescent="0.2">
-      <c r="S73" s="5"/>
-      <c r="U73" s="5"/>
+      <c r="S73" s="6"/>
+      <c r="U73" s="6"/>
     </row>
     <row r="74" spans="19:21" x14ac:dyDescent="0.2">
-      <c r="S74" s="5"/>
-      <c r="U74" s="5"/>
+      <c r="S74" s="6"/>
+      <c r="U74" s="6"/>
     </row>
     <row r="75" spans="19:21" x14ac:dyDescent="0.2">
-      <c r="S75" s="5"/>
-      <c r="U75" s="5"/>
+      <c r="S75" s="6"/>
+      <c r="U75" s="6"/>
     </row>
     <row r="76" spans="19:21" x14ac:dyDescent="0.2">
-      <c r="S76" s="5"/>
-      <c r="U76" s="5"/>
+      <c r="S76" s="6"/>
+      <c r="U76" s="6"/>
     </row>
     <row r="77" spans="19:21" x14ac:dyDescent="0.2">
-      <c r="S77" s="5"/>
-      <c r="U77" s="5"/>
+      <c r="S77" s="6"/>
+      <c r="U77" s="6"/>
     </row>
     <row r="78" spans="19:21" x14ac:dyDescent="0.2">
-      <c r="S78" s="5"/>
-      <c r="U78" s="5"/>
+      <c r="S78" s="6"/>
+      <c r="U78" s="6"/>
     </row>
     <row r="79" spans="19:21" x14ac:dyDescent="0.2">
-      <c r="S79" s="5"/>
-      <c r="U79" s="5"/>
+      <c r="S79" s="6"/>
+      <c r="U79" s="6"/>
     </row>
     <row r="80" spans="19:21" x14ac:dyDescent="0.2">
-      <c r="S80" s="5"/>
-      <c r="U80" s="5"/>
+      <c r="S80" s="6"/>
+      <c r="U80" s="6"/>
     </row>
     <row r="81" spans="19:21" x14ac:dyDescent="0.2">
-      <c r="S81" s="5"/>
-      <c r="U81" s="5"/>
+      <c r="S81" s="6"/>
+      <c r="U81" s="6"/>
     </row>
     <row r="82" spans="19:21" x14ac:dyDescent="0.2">
-      <c r="S82" s="5"/>
-      <c r="U82" s="5"/>
+      <c r="S82" s="6"/>
+      <c r="U82" s="6"/>
     </row>
     <row r="83" spans="19:21" x14ac:dyDescent="0.2">
-      <c r="S83" s="5"/>
-      <c r="U83" s="5"/>
+      <c r="S83" s="6"/>
+      <c r="U83" s="6"/>
     </row>
     <row r="84" spans="19:21" x14ac:dyDescent="0.2">
-      <c r="S84" s="5"/>
-      <c r="U84" s="5"/>
+      <c r="S84" s="6"/>
+      <c r="U84" s="6"/>
     </row>
     <row r="85" spans="19:21" x14ac:dyDescent="0.2">
-      <c r="S85" s="5"/>
-      <c r="U85" s="5"/>
+      <c r="S85" s="6"/>
+      <c r="U85" s="6"/>
     </row>
     <row r="86" spans="19:21" x14ac:dyDescent="0.2">
-      <c r="S86" s="5"/>
-      <c r="U86" s="5"/>
+      <c r="S86" s="6"/>
+      <c r="U86" s="6"/>
     </row>
     <row r="87" spans="19:21" x14ac:dyDescent="0.2">
-      <c r="S87" s="5"/>
-      <c r="U87" s="5"/>
+      <c r="S87" s="6"/>
+      <c r="U87" s="6"/>
     </row>
     <row r="88" spans="19:21" x14ac:dyDescent="0.2">
-      <c r="U88" s="5"/>
+      <c r="U88" s="6"/>
     </row>
     <row r="89" spans="19:21" x14ac:dyDescent="0.2">
-      <c r="U89" s="5"/>
+      <c r="U89" s="6"/>
     </row>
     <row r="90" spans="19:21" x14ac:dyDescent="0.2">
-      <c r="U90" s="5"/>
+      <c r="U90" s="6"/>
     </row>
     <row r="91" spans="19:21" x14ac:dyDescent="0.2">
-      <c r="U91" s="5"/>
+      <c r="U91" s="6"/>
     </row>
     <row r="92" spans="19:21" x14ac:dyDescent="0.2">
-      <c r="U92" s="5"/>
+      <c r="U92" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3077,7 +3153,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E6" t="s">
         <v>24</v>
@@ -3089,25 +3165,25 @@
         <v>26</v>
       </c>
       <c r="H6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="K6" t="s">
         <v>27</v>
       </c>
       <c r="L6" t="s">
+        <v>30</v>
+      </c>
+      <c r="M6" t="s">
         <v>31</v>
       </c>
-      <c r="M6" t="s">
-        <v>32</v>
-      </c>
       <c r="N6" t="s">
+        <v>28</v>
+      </c>
+      <c r="O6" t="s">
         <v>29</v>
-      </c>
-      <c r="O6" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.2">
@@ -3115,12 +3191,12 @@
         <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="7">
         <v>1.9999999999999999E-7</v>
       </c>
       <c r="F7">
@@ -3163,7 +3239,7 @@
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="7">
         <v>1.9999999999999999E-7</v>
       </c>
       <c r="F8">
@@ -3207,7 +3283,7 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
         <v>24</v>
@@ -3219,25 +3295,25 @@
         <v>26</v>
       </c>
       <c r="H5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K5" t="s">
         <v>27</v>
       </c>
       <c r="L5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M5" t="s">
         <v>31</v>
       </c>
-      <c r="M5" t="s">
-        <v>32</v>
-      </c>
       <c r="N5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O5" t="s">
         <v>29</v>
-      </c>
-      <c r="O5" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.2">
@@ -3247,7 +3323,7 @@
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="7">
         <v>1.9999999999999999E-7</v>
       </c>
       <c r="F6">
@@ -3287,7 +3363,7 @@
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="7">
         <v>1.9999999999999999E-7</v>
       </c>
       <c r="F7">
@@ -3313,14 +3389,1070 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B5D53CE-BD7A-6748-ADA6-17B85FC90549}">
-  <dimension ref="A1"/>
+  <dimension ref="C3:Q27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="17" max="17" width="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <v>800</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L5" t="s">
+        <v>36</v>
+      </c>
+      <c r="M5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N5" t="s">
+        <v>31</v>
+      </c>
+      <c r="O5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P5" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="7">
+        <v>1.9999999999999999E-7</v>
+      </c>
+      <c r="G6">
+        <v>0.01</v>
+      </c>
+      <c r="H6">
+        <v>16161</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6">
+        <v>3</v>
+      </c>
+      <c r="L6">
+        <v>-12541.630563999999</v>
+      </c>
+      <c r="M6">
+        <v>-1.0200000000000001E-2</v>
+      </c>
+      <c r="N6">
+        <v>-0.12479999999999999</v>
+      </c>
+      <c r="O6">
+        <f>AVERAGE(M6:N6)</f>
+        <v>-6.7500000000000004E-2</v>
+      </c>
+      <c r="P6" s="3">
+        <f t="shared" ref="P6" si="0">L7-L6</f>
+        <v>-458.45270160000109</v>
+      </c>
+      <c r="Q6" s="2">
+        <f>L7-(L6-460.15205)</f>
+        <v>1.6993483999995078</v>
+      </c>
+    </row>
+    <row r="7" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="7">
+        <v>1.9999999999999999E-7</v>
+      </c>
+      <c r="G7">
+        <v>0.01</v>
+      </c>
+      <c r="H7">
+        <v>16161</v>
+      </c>
+      <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="J7">
+        <v>3</v>
+      </c>
+      <c r="L7">
+        <v>-13000.0832656</v>
+      </c>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="2"/>
+    </row>
+    <row r="8" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="F8" s="7"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="2"/>
+    </row>
+    <row r="9" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>700</v>
+      </c>
+      <c r="E9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J9" t="s">
+        <v>40</v>
+      </c>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="2"/>
+    </row>
+    <row r="10" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="7">
+        <v>1.9999999999999999E-7</v>
+      </c>
+      <c r="G10">
+        <v>0.01</v>
+      </c>
+      <c r="H10">
+        <v>16161</v>
+      </c>
+      <c r="I10">
+        <v>5</v>
+      </c>
+      <c r="J10">
+        <v>3</v>
+      </c>
+      <c r="L10">
+        <v>-12541.619888499999</v>
+      </c>
+      <c r="M10">
+        <v>-1.2500000000000001E-2</v>
+      </c>
+      <c r="N10">
+        <v>-0.1229</v>
+      </c>
+      <c r="O10">
+        <f t="shared" ref="O7:O14" si="1">AVERAGE(M10:N10)</f>
+        <v>-6.7699999999999996E-2</v>
+      </c>
+      <c r="P10" s="3">
+        <f t="shared" ref="P7:P14" si="2">L11-L10</f>
+        <v>-458.44806570000037</v>
+      </c>
+      <c r="Q10" s="2">
+        <f t="shared" ref="Q7:Q14" si="3">L11-(L10-460.15205)</f>
+        <v>1.7039843000002293</v>
+      </c>
+    </row>
+    <row r="11" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" s="7">
+        <v>1.9999999999999999E-7</v>
+      </c>
+      <c r="G11">
+        <v>0.01</v>
+      </c>
+      <c r="H11">
+        <v>16161</v>
+      </c>
+      <c r="I11">
+        <v>5</v>
+      </c>
+      <c r="J11">
+        <v>3</v>
+      </c>
+      <c r="L11">
+        <v>-13000.0679542</v>
+      </c>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="2"/>
+    </row>
+    <row r="12" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="P12" s="3"/>
+      <c r="Q12" s="2"/>
+    </row>
+    <row r="13" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <v>600</v>
+      </c>
+      <c r="E13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" t="s">
+        <v>39</v>
+      </c>
+      <c r="I13" t="s">
+        <v>38</v>
+      </c>
+      <c r="J13" t="s">
+        <v>40</v>
+      </c>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="2"/>
+    </row>
+    <row r="14" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" s="7">
+        <v>1.9999999999999999E-7</v>
+      </c>
+      <c r="G14">
+        <v>0.01</v>
+      </c>
+      <c r="H14">
+        <v>16161</v>
+      </c>
+      <c r="I14">
+        <v>5</v>
+      </c>
+      <c r="J14">
+        <v>3</v>
+      </c>
+      <c r="L14">
+        <v>-12541.577488999999</v>
+      </c>
+      <c r="M14">
+        <v>0.20469999999999999</v>
+      </c>
+      <c r="N14">
+        <v>-0.34039999999999998</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="1"/>
+        <v>-6.7849999999999994E-2</v>
+      </c>
+      <c r="P14" s="3">
+        <f t="shared" si="2"/>
+        <v>-458.44231589999981</v>
+      </c>
+      <c r="Q14" s="2">
+        <f t="shared" si="3"/>
+        <v>1.7097341000007873</v>
+      </c>
+    </row>
+    <row r="15" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" s="7">
+        <v>1.9999999999999999E-7</v>
+      </c>
+      <c r="G15">
+        <v>0.01</v>
+      </c>
+      <c r="H15">
+        <v>16161</v>
+      </c>
+      <c r="I15">
+        <v>5</v>
+      </c>
+      <c r="J15">
+        <v>3</v>
+      </c>
+      <c r="L15">
+        <v>-13000.019804899999</v>
+      </c>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="8"/>
+    </row>
+    <row r="16" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="F16" s="7"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="8"/>
+    </row>
+    <row r="17" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C17">
+        <v>500</v>
+      </c>
+      <c r="E17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" t="s">
+        <v>39</v>
+      </c>
+      <c r="I17" t="s">
+        <v>38</v>
+      </c>
+      <c r="J17" t="s">
+        <v>40</v>
+      </c>
+      <c r="L17" t="s">
+        <v>36</v>
+      </c>
+      <c r="M17" t="s">
+        <v>30</v>
+      </c>
+      <c r="N17" t="s">
+        <v>31</v>
+      </c>
+      <c r="O17" t="s">
+        <v>28</v>
+      </c>
+      <c r="P17" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" s="7">
+        <v>1.9999999999999999E-7</v>
+      </c>
+      <c r="G18">
+        <v>0.01</v>
+      </c>
+      <c r="H18">
+        <v>16161</v>
+      </c>
+      <c r="I18">
+        <v>5</v>
+      </c>
+      <c r="J18">
+        <v>3</v>
+      </c>
+      <c r="L18">
+        <v>-12541.5315753</v>
+      </c>
+      <c r="M18">
+        <v>0.16830000000000001</v>
+      </c>
+      <c r="N18">
+        <v>-0.30309999999999998</v>
+      </c>
+      <c r="O18">
+        <f>AVERAGE(M18:N18)</f>
+        <v>-6.7399999999999988E-2</v>
+      </c>
+      <c r="P18" s="3">
+        <f t="shared" ref="P18:P19" si="4">L19-L18</f>
+        <v>-458.43842530000074</v>
+      </c>
+      <c r="Q18" s="2">
+        <f>L19-(L18-460.15205)</f>
+        <v>1.7136246999998548</v>
+      </c>
+    </row>
+    <row r="19" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" s="7">
+        <v>1.9999999999999999E-7</v>
+      </c>
+      <c r="G19">
+        <v>0.01</v>
+      </c>
+      <c r="H19">
+        <v>16161</v>
+      </c>
+      <c r="I19">
+        <v>5</v>
+      </c>
+      <c r="J19">
+        <v>3</v>
+      </c>
+      <c r="L19">
+        <v>-12999.9700006</v>
+      </c>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="2"/>
+    </row>
+    <row r="20" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="Q20" s="2"/>
+    </row>
+    <row r="21" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C21">
+        <v>400</v>
+      </c>
+      <c r="E21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H21" t="s">
+        <v>39</v>
+      </c>
+      <c r="I21" t="s">
+        <v>38</v>
+      </c>
+      <c r="J21" t="s">
+        <v>40</v>
+      </c>
+      <c r="L21" t="s">
+        <v>36</v>
+      </c>
+      <c r="M21" t="s">
+        <v>30</v>
+      </c>
+      <c r="N21" t="s">
+        <v>31</v>
+      </c>
+      <c r="O21" t="s">
+        <v>28</v>
+      </c>
+      <c r="P21" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="F22" s="7">
+        <v>1.9999999999999999E-7</v>
+      </c>
+      <c r="G22">
+        <v>0.01</v>
+      </c>
+      <c r="H22">
+        <v>16161</v>
+      </c>
+      <c r="I22">
+        <v>5</v>
+      </c>
+      <c r="J22">
+        <v>3</v>
+      </c>
+      <c r="L22">
+        <v>-12539.3333043</v>
+      </c>
+      <c r="M22">
+        <v>0.21859999999999999</v>
+      </c>
+      <c r="N22">
+        <v>-0.3599</v>
+      </c>
+      <c r="O22">
+        <f>AVERAGE(M22:N22)</f>
+        <v>-7.0650000000000004E-2</v>
+      </c>
+      <c r="P22" s="3">
+        <f t="shared" ref="P22:P23" si="5">L23-L22</f>
+        <v>-458.28810820000035</v>
+      </c>
+      <c r="Q22" s="2">
+        <f>L23-(L22-460.15205)</f>
+        <v>1.8639418000002479</v>
+      </c>
+    </row>
+    <row r="23" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23">
+        <v>2</v>
+      </c>
+      <c r="F23" s="7">
+        <v>1.9999999999999999E-7</v>
+      </c>
+      <c r="G23">
+        <v>0.01</v>
+      </c>
+      <c r="H23">
+        <v>16161</v>
+      </c>
+      <c r="I23">
+        <v>5</v>
+      </c>
+      <c r="J23">
+        <v>3</v>
+      </c>
+      <c r="L23">
+        <v>-12997.621412500001</v>
+      </c>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="2"/>
+    </row>
+    <row r="24" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="Q24" s="2"/>
+    </row>
+    <row r="25" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C25">
+        <v>300</v>
+      </c>
+      <c r="E25" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" t="s">
+        <v>24</v>
+      </c>
+      <c r="G25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H25" t="s">
+        <v>39</v>
+      </c>
+      <c r="I25" t="s">
+        <v>38</v>
+      </c>
+      <c r="J25" t="s">
+        <v>40</v>
+      </c>
+      <c r="L25" t="s">
+        <v>36</v>
+      </c>
+      <c r="M25" t="s">
+        <v>30</v>
+      </c>
+      <c r="N25" t="s">
+        <v>31</v>
+      </c>
+      <c r="O25" t="s">
+        <v>28</v>
+      </c>
+      <c r="P25" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26">
+        <v>3</v>
+      </c>
+      <c r="F26" s="7">
+        <v>1.9999999999999999E-7</v>
+      </c>
+      <c r="G26">
+        <v>0.01</v>
+      </c>
+      <c r="H26">
+        <v>16161</v>
+      </c>
+      <c r="I26">
+        <v>5</v>
+      </c>
+      <c r="J26">
+        <v>3</v>
+      </c>
+      <c r="L26">
+        <v>-12505.918188899999</v>
+      </c>
+      <c r="M26">
+        <v>-0.12809999999999999</v>
+      </c>
+      <c r="N26">
+        <v>-4.7699999999999999E-2</v>
+      </c>
+      <c r="O26">
+        <f>AVERAGE(M26:N26)</f>
+        <v>-8.7899999999999992E-2</v>
+      </c>
+      <c r="P26" s="3">
+        <f t="shared" ref="P26:P27" si="6">L27-L26</f>
+        <v>-456.8089899000006</v>
+      </c>
+      <c r="Q26" s="2">
+        <f>L27-(L26-460.15205)</f>
+        <v>3.3430601000000024</v>
+      </c>
+    </row>
+    <row r="27" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="F27" s="7">
+        <v>1.9999999999999999E-7</v>
+      </c>
+      <c r="G27">
+        <v>0.01</v>
+      </c>
+      <c r="H27">
+        <v>16161</v>
+      </c>
+      <c r="I27">
+        <v>5</v>
+      </c>
+      <c r="J27">
+        <v>3</v>
+      </c>
+      <c r="L27">
+        <v>-12962.7271788</v>
+      </c>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC128D54-F998-7145-AF87-4CAEE58A6435}">
+  <dimension ref="B3:Q14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" t="s">
+        <v>43</v>
+      </c>
+      <c r="L3" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1.9999999999999999E-7</v>
+      </c>
+      <c r="F4">
+        <v>0.01</v>
+      </c>
+      <c r="G4">
+        <v>881</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <v>700</v>
+      </c>
+      <c r="L4">
+        <v>-50166.493196900003</v>
+      </c>
+      <c r="P4" s="3">
+        <f t="shared" ref="P4" si="0">L5-L4</f>
+        <v>-458.7277202999976</v>
+      </c>
+      <c r="Q4" s="2">
+        <f>L5-(L4-460.15205)</f>
+        <v>1.4243296999993618</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5" s="7">
+        <v>1.9999999999999999E-7</v>
+      </c>
+      <c r="F5">
+        <v>0.01</v>
+      </c>
+      <c r="G5">
+        <v>881</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
+      <c r="J5">
+        <v>700</v>
+      </c>
+      <c r="L5">
+        <v>-50625.2209172</v>
+      </c>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="2"/>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" t="s">
+        <v>40</v>
+      </c>
+      <c r="L7" t="s">
+        <v>36</v>
+      </c>
+      <c r="M7" t="s">
+        <v>30</v>
+      </c>
+      <c r="N7" t="s">
+        <v>31</v>
+      </c>
+      <c r="O7" t="s">
+        <v>28</v>
+      </c>
+      <c r="P7" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="7">
+        <v>1.9999999999999999E-7</v>
+      </c>
+      <c r="F8">
+        <v>0.01</v>
+      </c>
+      <c r="G8">
+        <v>441</v>
+      </c>
+      <c r="H8">
+        <v>5</v>
+      </c>
+      <c r="I8">
+        <v>3</v>
+      </c>
+      <c r="J8">
+        <v>700</v>
+      </c>
+      <c r="P8" s="3">
+        <f t="shared" ref="P8" si="1">L9-L8</f>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="2">
+        <f>L9-(L8-460.15205)</f>
+        <v>460.15204999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="7">
+        <v>1.9999999999999999E-7</v>
+      </c>
+      <c r="F9">
+        <v>0.01</v>
+      </c>
+      <c r="G9">
+        <v>441</v>
+      </c>
+      <c r="H9">
+        <v>5</v>
+      </c>
+      <c r="I9">
+        <v>3</v>
+      </c>
+      <c r="J9">
+        <v>700</v>
+      </c>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="2"/>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" t="s">
+        <v>39</v>
+      </c>
+      <c r="H12" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" t="s">
+        <v>40</v>
+      </c>
+      <c r="J12" t="s">
+        <v>43</v>
+      </c>
+      <c r="L12" t="s">
+        <v>36</v>
+      </c>
+      <c r="M12" t="s">
+        <v>30</v>
+      </c>
+      <c r="N12" t="s">
+        <v>31</v>
+      </c>
+      <c r="O12" t="s">
+        <v>28</v>
+      </c>
+      <c r="P12" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13" s="7">
+        <v>1.9999999999999999E-7</v>
+      </c>
+      <c r="F13">
+        <v>0.01</v>
+      </c>
+      <c r="G13">
+        <v>881</v>
+      </c>
+      <c r="H13">
+        <v>5</v>
+      </c>
+      <c r="I13">
+        <v>3</v>
+      </c>
+      <c r="J13">
+        <v>700</v>
+      </c>
+      <c r="L13">
+        <v>-50166.493196900003</v>
+      </c>
+      <c r="P13" s="3">
+        <f t="shared" ref="P13" si="2">L14-L13</f>
+        <v>50166.493196900003</v>
+      </c>
+      <c r="Q13" s="2">
+        <f>L14-(L13-460.15205)</f>
+        <v>50626.6452469</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14" s="7">
+        <v>1.9999999999999999E-7</v>
+      </c>
+      <c r="F14">
+        <v>0.01</v>
+      </c>
+      <c r="G14">
+        <v>881</v>
+      </c>
+      <c r="H14">
+        <v>5</v>
+      </c>
+      <c r="I14">
+        <v>3</v>
+      </c>
+      <c r="J14">
+        <v>700</v>
+      </c>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated analysis excel file
</commit_message>
<xml_diff>
--- a/data/Supported Graphene Analysis.xlsx
+++ b/data/Supported Graphene Analysis.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinkrempl/Documents/TRI ORR/Data/DFT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF91AC9-A8ED-8041-992E-8A2DDD087076}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D89C256-2214-AD43-BA69-86430519DFAF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="5" xr2:uid="{4048BA77-A555-4A4B-8B58-A70623B0558E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="6" xr2:uid="{4048BA77-A555-4A4B-8B58-A70623B0558E}"/>
   </bookViews>
   <sheets>
     <sheet name="Lattice matching" sheetId="1" r:id="rId1"/>
-    <sheet name="kpts" sheetId="2" r:id="rId2"/>
-    <sheet name="vacuum" sheetId="4" r:id="rId3"/>
-    <sheet name="layers" sheetId="5" r:id="rId4"/>
-    <sheet name="pwcutoff " sheetId="3" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
+    <sheet name="surfaces" sheetId="7" r:id="rId2"/>
+    <sheet name="kpts" sheetId="2" r:id="rId3"/>
+    <sheet name="vacuum" sheetId="4" r:id="rId4"/>
+    <sheet name="layers" sheetId="5" r:id="rId5"/>
+    <sheet name="pwcutoff " sheetId="3" r:id="rId6"/>
+    <sheet name="coverage" sheetId="6" r:id="rId7"/>
+    <sheet name="other" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="53">
   <si>
     <t>001</t>
   </si>
@@ -164,10 +166,31 @@
     <t>pw cutoff</t>
   </si>
   <si>
-    <t>4x4</t>
-  </si>
-  <si>
     <t>2x2 trifold ontop</t>
+  </si>
+  <si>
+    <t>hcp11m20</t>
+  </si>
+  <si>
+    <t>magmoms</t>
+  </si>
+  <si>
+    <t>ooh</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>3x3 trifold ontop</t>
+  </si>
+  <si>
+    <t>Mo bcc 111</t>
+  </si>
+  <si>
+    <t>Co hcp11m20</t>
+  </si>
+  <si>
+    <t>4x4 trifold ontop</t>
   </si>
 </sst>
 </file>
@@ -542,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F803174-99F6-A54F-9056-59F666BF7275}">
-  <dimension ref="B2:L47"/>
+  <dimension ref="B2:N47"/>
   <sheetViews>
     <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -561,7 +584,7 @@
     <col min="12" max="12" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -596,12 +619,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -633,7 +656,7 @@
         <v>59.999999999999901</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>100</v>
       </c>
@@ -665,7 +688,7 @@
         <v>0.29264690570200003</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>101</v>
       </c>
@@ -696,8 +719,12 @@
       <c r="K7" s="5">
         <v>5.8201933957306502E-2</v>
       </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="N7">
+        <f>9*H5</f>
+        <v>47.394076187765435</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>110</v>
       </c>
@@ -728,8 +755,16 @@
       <c r="K8" s="5">
         <v>1.4210854715202001E-14</v>
       </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="M8">
+        <f>F5*16</f>
+        <v>39.8418992</v>
+      </c>
+      <c r="N8">
+        <f>M8/G33</f>
+        <v>4.4562293864476237</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>210</v>
       </c>
@@ -761,7 +796,7 @@
         <v>0.36505132780217697</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>13</v>
       </c>
@@ -772,7 +807,7 @@
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>100</v>
       </c>
@@ -804,7 +839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>110</v>
       </c>
@@ -836,7 +871,7 @@
         <v>2.8421709430404001E-14</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>111</v>
       </c>
@@ -868,7 +903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>221</v>
       </c>
@@ -900,7 +935,7 @@
         <v>1.4210854715202001E-14</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B15">
         <v>322</v>
       </c>
@@ -932,7 +967,7 @@
         <v>2.25564187795868E-2</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B16">
         <v>332</v>
       </c>
@@ -1842,11 +1877,137 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FA35E21-EE8E-B845-B52D-629E949D26F0}">
+  <dimension ref="B3:R5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" t="s">
+        <v>30</v>
+      </c>
+      <c r="P3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>28</v>
+      </c>
+      <c r="R3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="F4">
+        <v>0.01</v>
+      </c>
+      <c r="G4">
+        <v>400</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <v>931</v>
+      </c>
+      <c r="K4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="e">
+        <f>AVERAGE(O4:P4)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R4" s="3">
+        <f t="shared" ref="R4:R5" si="0">M5-M4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="7">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="F5">
+        <v>0.01</v>
+      </c>
+      <c r="G5">
+        <v>800</v>
+      </c>
+      <c r="H5">
+        <v>10</v>
+      </c>
+      <c r="I5">
+        <v>6</v>
+      </c>
+      <c r="J5">
+        <v>931</v>
+      </c>
+      <c r="R5" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA11F605-3F2C-8949-A07B-2C4748B8A05E}">
   <dimension ref="B2:U92"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3133,7 +3294,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90FF3DB4-F55F-0B49-AD2B-5509731BE8F4}">
   <dimension ref="B4:O8"/>
   <sheetViews>
@@ -3263,7 +3424,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E90C5FF2-D8D0-4349-80EC-68F7DB260FDB}">
   <dimension ref="B3:O7"/>
   <sheetViews>
@@ -3387,12 +3548,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B5D53CE-BD7A-6748-ADA6-17B85FC90549}">
   <dimension ref="C3:Q27"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4112,12 +4273,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC128D54-F998-7145-AF87-4CAEE58A6435}">
-  <dimension ref="B3:Q14"/>
+  <dimension ref="B3:Q21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4171,7 +4332,7 @@
         <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -4195,15 +4356,15 @@
         <v>700</v>
       </c>
       <c r="L4">
-        <v>-50166.493196900003</v>
+        <v>-50166.479172200001</v>
       </c>
       <c r="P4" s="3">
         <f t="shared" ref="P4" si="0">L5-L4</f>
-        <v>-458.7277202999976</v>
+        <v>-458.74174499999936</v>
       </c>
       <c r="Q4" s="2">
         <f>L5-(L4-460.15205)</f>
-        <v>1.4243296999993618</v>
+        <v>1.4103049999976065</v>
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.2">
@@ -4242,7 +4403,7 @@
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D7" t="s">
         <v>33</v>
@@ -4285,6 +4446,9 @@
       <c r="B8" t="s">
         <v>19</v>
       </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
       <c r="D8">
         <v>1</v>
       </c>
@@ -4295,7 +4459,7 @@
         <v>0.01</v>
       </c>
       <c r="G8">
-        <v>441</v>
+        <v>551</v>
       </c>
       <c r="H8">
         <v>5</v>
@@ -4306,19 +4470,25 @@
       <c r="J8">
         <v>700</v>
       </c>
+      <c r="L8">
+        <v>-112873.85752200001</v>
+      </c>
       <c r="P8" s="3">
         <f t="shared" ref="P8" si="1">L9-L8</f>
-        <v>0</v>
+        <v>-459.49735199999122</v>
       </c>
       <c r="Q8" s="2">
         <f>L9-(L8-460.15205)</f>
-        <v>460.15204999999997</v>
+        <v>0.65469800001301337</v>
       </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>20</v>
       </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
       <c r="D9">
         <v>1</v>
       </c>
@@ -4329,7 +4499,7 @@
         <v>0.01</v>
       </c>
       <c r="G9">
-        <v>441</v>
+        <v>551</v>
       </c>
       <c r="H9">
         <v>5</v>
@@ -4340,12 +4510,15 @@
       <c r="J9">
         <v>700</v>
       </c>
+      <c r="L9">
+        <v>-113333.354874</v>
+      </c>
       <c r="P9" s="3"/>
       <c r="Q9" s="2"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D12" t="s">
         <v>33</v>
@@ -4391,6 +4564,9 @@
       <c r="B13" t="s">
         <v>19</v>
       </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
       <c r="D13">
         <v>3</v>
       </c>
@@ -4413,21 +4589,20 @@
         <v>700</v>
       </c>
       <c r="L13">
-        <v>-50166.493196900003</v>
+        <v>-50166.479172200001</v>
       </c>
       <c r="P13" s="3">
         <f t="shared" ref="P13" si="2">L14-L13</f>
-        <v>50166.493196900003</v>
-      </c>
-      <c r="Q13" s="2">
-        <f>L14-(L13-460.15205)</f>
-        <v>50626.6452469</v>
+        <v>-459.13675579999835</v>
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>20</v>
       </c>
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
       <c r="D14">
         <v>3</v>
       </c>
@@ -4449,8 +4624,223 @@
       <c r="J14">
         <v>700</v>
       </c>
+      <c r="L14">
+        <v>-50625.615927999999</v>
+      </c>
       <c r="P14" s="3"/>
-      <c r="Q14" s="2"/>
+      <c r="Q14" s="2">
+        <f>L14-(L13-460.15205)</f>
+        <v>1.0152941999986069</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" s="7">
+        <v>1.9999999999999999E-7</v>
+      </c>
+      <c r="F15">
+        <v>0.01</v>
+      </c>
+      <c r="G15">
+        <v>881</v>
+      </c>
+      <c r="H15">
+        <v>5</v>
+      </c>
+      <c r="I15">
+        <v>3</v>
+      </c>
+      <c r="J15">
+        <v>700</v>
+      </c>
+      <c r="L15">
+        <v>-51066.2000568</v>
+      </c>
+      <c r="Q15" s="2">
+        <f>L15-(L13-2*443.674358207704-16.47769)</f>
+        <v>4.1055218154069735</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" s="7">
+        <v>1.9999999999999999E-7</v>
+      </c>
+      <c r="F16">
+        <v>0.01</v>
+      </c>
+      <c r="G16">
+        <v>881</v>
+      </c>
+      <c r="H16">
+        <v>5</v>
+      </c>
+      <c r="I16">
+        <v>3</v>
+      </c>
+      <c r="J16">
+        <v>700</v>
+      </c>
+      <c r="L16">
+        <v>-50607.445810999998</v>
+      </c>
+      <c r="Q16" s="2">
+        <f>L16-(L13-443.674358207704)</f>
+        <v>2.7077194077064632</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" t="s">
+        <v>39</v>
+      </c>
+      <c r="H19" t="s">
+        <v>38</v>
+      </c>
+      <c r="I19" t="s">
+        <v>40</v>
+      </c>
+      <c r="J19" t="s">
+        <v>43</v>
+      </c>
+      <c r="L19" t="s">
+        <v>36</v>
+      </c>
+      <c r="M19" t="s">
+        <v>30</v>
+      </c>
+      <c r="N19" t="s">
+        <v>31</v>
+      </c>
+      <c r="O19" t="s">
+        <v>28</v>
+      </c>
+      <c r="P19" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" s="7">
+        <v>1.9999999999999999E-7</v>
+      </c>
+      <c r="F20">
+        <v>0.01</v>
+      </c>
+      <c r="G20">
+        <v>551</v>
+      </c>
+      <c r="H20">
+        <v>5</v>
+      </c>
+      <c r="I20">
+        <v>3</v>
+      </c>
+      <c r="J20">
+        <v>700</v>
+      </c>
+      <c r="P20" s="3">
+        <f>L21-L20</f>
+        <v>0</v>
+      </c>
+      <c r="Q20" s="2">
+        <f>L21-(L20-460.15205)</f>
+        <v>460.15204999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" s="7">
+        <v>1.9999999999999999E-7</v>
+      </c>
+      <c r="F21">
+        <v>0.01</v>
+      </c>
+      <c r="G21">
+        <v>551</v>
+      </c>
+      <c r="H21">
+        <v>5</v>
+      </c>
+      <c r="I21">
+        <v>3</v>
+      </c>
+      <c r="J21">
+        <v>700</v>
+      </c>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{578A1A54-CAA0-D146-B899-917B401DB322}">
+  <dimension ref="B4:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>